<commit_message>
Updated game_levels.xlsx and rounds_config.json
</commit_message>
<xml_diff>
--- a/tools/game_levels.xlsx
+++ b/tools/game_levels.xlsx
@@ -756,13 +756,13 @@
     <t>notify_gov_statement_text</t>
   </si>
   <si>
-    <t>Die Folgen des Vulkanausbruchs sind stark spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, muss weiterhin und zu jeder Zeit die Spezialbrille getragen und täglich das Bad genommen werden. Diese Schutzmassnahmen sind für alle verpflichtend.</t>
-  </si>
-  <si>
-    <t>Die Folgen des Vulkanausbruchs sind weiterhin spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, wird weiterhin empfohlen, zu jeder Zeit die Spezialbrille zu tragen und täglich das Bad zu nehmen. Diese Schutzmassnahmen werden allen empfohlen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Folgen des Vulkanausbruchs haben nachgelassen. Dennoch kann man sich immer noch infizieren, andere anstecken und sterben. Die Regierung hat diese Risiken gegen die Einschränkungen durch die Schutzmassnahmen abgewogen und gibt nun keine Empfehlungen mehr ab. Ob man die Spezialbrille trägt oder das tägliche Bad einnimmt, ist jedem Mika selbst überlassen. </t>
+    <t>Die Folgen des Vulkanausbruchs sind stark spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, muss weiterhin und zu jeder Zeit die Spezialbrille getragen und täglich das Bad genommen werden. Diese Schutzmassnahmen sind für alle verpflichtend. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
+  </si>
+  <si>
+    <t>Die Folgen des Vulkanausbruchs sind weiterhin spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, wird weiterhin empfohlen, zu jeder Zeit die Spezialbrille zu tragen und täglich das Bad zu nehmen. Diese Schutzmassnahmen werden allen empfohlen. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
+  </si>
+  <si>
+    <t>Die Folgen des Vulkanausbruchs haben nachgelassen. Dennoch kann man sich immer noch infizieren, andere anstecken und sterben. Die Regierung hat diese Risiken gegen die Einschränkungen durch die Schutzmassnahmen abgewogen und gibt nun keine Empfehlungen mehr ab. Ob man die Spezialbrille trägt oder das tägliche Bad einnimmt, ist jedem Mika selbst überlassen. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
   </si>
   <si>
     <t>40% of ingroup NPCs wear a hat and a necklace; 60% wear only a hat</t>
@@ -13260,37 +13260,29 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="I57:N57"/>
-    <mergeCell ref="I58:N58"/>
-    <mergeCell ref="I42:N42"/>
-    <mergeCell ref="I44:N44"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="I48:N48"/>
-    <mergeCell ref="I50:N50"/>
-    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I26:N26"/>
+    <mergeCell ref="I27:N27"/>
+    <mergeCell ref="I28:N28"/>
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I40:N40"/>
+    <mergeCell ref="I42:N42"/>
+    <mergeCell ref="I57:N57"/>
+    <mergeCell ref="I58:N58"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="I48:N48"/>
+    <mergeCell ref="I50:N50"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="J54:N54"/>
     <mergeCell ref="I56:N56"/>
-    <mergeCell ref="J54:N54"/>
-    <mergeCell ref="C56:H56"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="C44:H44"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C57:H57"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="C78:H78"/>
-    <mergeCell ref="C79:H79"/>
-    <mergeCell ref="I80:N80"/>
-    <mergeCell ref="I81:N81"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:N1"/>
@@ -13320,13 +13312,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I26:N26"/>
-    <mergeCell ref="I27:N27"/>
-    <mergeCell ref="I28:N28"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="C28:H28"/>
     <mergeCell ref="C29:H29"/>
@@ -13334,8 +13319,23 @@
     <mergeCell ref="C31:H31"/>
     <mergeCell ref="C32:H32"/>
     <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="C52:H52"/>
     <mergeCell ref="C80:H80"/>
     <mergeCell ref="C81:H81"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="C56:H56"/>
+    <mergeCell ref="C57:H57"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="C79:H79"/>
+    <mergeCell ref="I80:N80"/>
+    <mergeCell ref="I81:N81"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19169,37 +19169,29 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="I57:N57"/>
-    <mergeCell ref="I58:N58"/>
-    <mergeCell ref="I42:N42"/>
-    <mergeCell ref="I44:N44"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="I48:N48"/>
-    <mergeCell ref="I50:N50"/>
-    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I26:N26"/>
+    <mergeCell ref="I27:N27"/>
+    <mergeCell ref="I28:N28"/>
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I40:N40"/>
+    <mergeCell ref="I42:N42"/>
+    <mergeCell ref="I57:N57"/>
+    <mergeCell ref="I58:N58"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="I48:N48"/>
+    <mergeCell ref="I50:N50"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="J54:N54"/>
     <mergeCell ref="I56:N56"/>
-    <mergeCell ref="J54:N54"/>
-    <mergeCell ref="C56:H56"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="C44:H44"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C57:H57"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="C76:H76"/>
-    <mergeCell ref="C77:H77"/>
-    <mergeCell ref="I78:N78"/>
-    <mergeCell ref="I79:N79"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:N1"/>
@@ -19229,13 +19221,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I26:N26"/>
-    <mergeCell ref="I27:N27"/>
-    <mergeCell ref="I28:N28"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="C28:H28"/>
     <mergeCell ref="C29:H29"/>
@@ -19243,8 +19228,23 @@
     <mergeCell ref="C31:H31"/>
     <mergeCell ref="C32:H32"/>
     <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="C52:H52"/>
     <mergeCell ref="C78:H78"/>
     <mergeCell ref="C79:H79"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="C56:H56"/>
+    <mergeCell ref="C57:H57"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C76:H76"/>
+    <mergeCell ref="C77:H77"/>
+    <mergeCell ref="I78:N78"/>
+    <mergeCell ref="I79:N79"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated game_levels.xlsx and rounds_config.json for post eruption discussions
</commit_message>
<xml_diff>
--- a/tools/game_levels.xlsx
+++ b/tools/game_levels.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="250">
   <si>
     <t>Feature</t>
   </si>
@@ -666,19 +666,7 @@
     <t>market_active_family</t>
   </si>
   <si>
-    <t>Textbox and scripted sequence: Group discussion how to deal with the new rules; player can make a decision timestamp</t>
-  </si>
-  <si>
-    <t>market_active_post_eruption_timestamp</t>
-  </si>
-  <si>
-    <t>Textbox and scripted sequence: Group discussion how to deal with the new rules; player can make a decision text</t>
-  </si>
-  <si>
-    <t>market_active_post_eruption_text</t>
-  </si>
-  <si>
-    <t>Dein Familienclan versammelt sich zur täglichen Abstimmung darüber, wie mit den neuen Regeln umgegangen werden soll. Da du ein Vollmitglied der Rothüte bist, darfst auch du abstimmen! Drücke die Leertaste, um fortzufahren.</t>
+    <t>market_active_post_eruption_family</t>
   </si>
   <si>
     <t>Gov statement timestamp</t>
@@ -742,6 +730,9 @@
   </si>
   <si>
     <t>market_active_friends</t>
+  </si>
+  <si>
+    <t>market_active_post_eruption_friends</t>
   </si>
   <si>
     <t>Game levels and features study 3b, v3 (no group version)</t>
@@ -2975,12 +2966,24 @@
       <c r="H64" s="15">
         <v>0.08333333333333333</v>
       </c>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
+      <c r="I64" s="16">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="J64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="L64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="M64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="N64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="9" t="s">
@@ -2999,184 +3002,140 @@
       <c r="H65" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
+      <c r="I65" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J65" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K65" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="L65" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="16">
-        <v>0.4166666666666667</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="16"/>
       <c r="J66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="K66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="L66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="M66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="N66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17" t="s">
         <v>221</v>
       </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="17"/>
       <c r="J67" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="L67" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="M67" s="17" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C68" s="14"/>
+      <c r="A68" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="12"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="K68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="L68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="M68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="N68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
+      <c r="I68" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="12"/>
     </row>
     <row r="69">
-      <c r="A69" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C69" s="14"/>
+      <c r="A69" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="12"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="K69" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="L69" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="M69" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="N69" s="17" t="s">
-        <v>228</v>
-      </c>
+      <c r="I69" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="12"/>
     </row>
     <row r="70">
-      <c r="A70" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="12"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
     </row>
     <row r="71">
-      <c r="A71" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="12"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
     </row>
     <row r="72">
       <c r="A72" s="37"/>
@@ -6917,14 +6876,6 @@
     <row r="1006">
       <c r="A1006" s="37"/>
       <c r="B1006" s="37"/>
-    </row>
-    <row r="1007">
-      <c r="A1007" s="37"/>
-      <c r="B1007" s="37"/>
-    </row>
-    <row r="1008">
-      <c r="A1008" s="37"/>
-      <c r="B1008" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="65">
@@ -6981,18 +6932,18 @@
     <mergeCell ref="J46:N46"/>
     <mergeCell ref="I47:N47"/>
     <mergeCell ref="I48:N48"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="I68:N68"/>
     <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="I70:N70"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="I71:N71"/>
+    <mergeCell ref="I69:N69"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="C42:H42"/>
     <mergeCell ref="C44:H44"/>
     <mergeCell ref="C46:H46"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C66:H66"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -7020,7 +6971,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
@@ -7636,13 +7587,13 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -8352,7 +8303,7 @@
         <v>174</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -8418,7 +8369,7 @@
         <v>183</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="8"/>
@@ -8485,7 +8436,7 @@
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
@@ -8576,7 +8527,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
@@ -8662,16 +8613,16 @@
         <v>210</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
@@ -8699,12 +8650,24 @@
       <c r="H64" s="36">
         <v>0.08333333333333333</v>
       </c>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
+      <c r="I64" s="16">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="J64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="L64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="M64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="N64" s="16">
+        <v>0.08333333333333333</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="9" t="s">
@@ -8718,189 +8681,145 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="17" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H65" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
+        <v>238</v>
+      </c>
+      <c r="I65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="16">
-        <v>0.4166666666666667</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="16"/>
       <c r="J66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="K66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="L66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="M66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="N66" s="16">
-        <v>0.08333333333333333</v>
+        <v>0.013888888888888888</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17" t="s">
         <v>221</v>
       </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="17"/>
       <c r="J67" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="L67" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="M67" s="17" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C68" s="14"/>
+      <c r="A68" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="12"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="K68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="L68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="M68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="N68" s="16">
-        <v>0.013888888888888888</v>
-      </c>
+      <c r="I68" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="12"/>
     </row>
     <row r="69">
-      <c r="A69" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C69" s="14"/>
+      <c r="A69" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="12"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="K69" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="L69" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="M69" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="N69" s="17" t="s">
-        <v>228</v>
-      </c>
+      <c r="I69" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="12"/>
     </row>
     <row r="70">
-      <c r="A70" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="12"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
     </row>
     <row r="71">
-      <c r="A71" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="12"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
     </row>
     <row r="72">
       <c r="A72" s="37"/>
@@ -12641,14 +12560,6 @@
     <row r="1006">
       <c r="A1006" s="37"/>
       <c r="B1006" s="37"/>
-    </row>
-    <row r="1007">
-      <c r="A1007" s="37"/>
-      <c r="B1007" s="37"/>
-    </row>
-    <row r="1008">
-      <c r="A1008" s="37"/>
-      <c r="B1008" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="66">
@@ -12706,18 +12617,18 @@
     <mergeCell ref="J46:N46"/>
     <mergeCell ref="I47:N47"/>
     <mergeCell ref="I48:N48"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="I68:N68"/>
     <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="I70:N70"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="I71:N71"/>
+    <mergeCell ref="I69:N69"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="C42:H42"/>
     <mergeCell ref="C44:H44"/>
     <mergeCell ref="C46:H46"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C66:H66"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -12745,7 +12656,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
@@ -12795,7 +12706,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>17</v>
@@ -13349,13 +13260,13 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -14043,7 +13954,7 @@
         <v>172</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -14065,7 +13976,7 @@
         <v>174</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -14087,7 +13998,7 @@
         <v>177</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="8"/>
@@ -14109,7 +14020,7 @@
         <v>180</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="8"/>
@@ -14125,13 +14036,13 @@
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>183</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="8"/>
@@ -14153,7 +14064,7 @@
         <v>186</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="8"/>
@@ -14319,7 +14230,7 @@
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
@@ -14413,10 +14324,10 @@
     </row>
     <row r="66">
       <c r="A66" s="13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="11"/>
@@ -14443,10 +14354,10 @@
     </row>
     <row r="67">
       <c r="A67" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="11"/>
@@ -14456,27 +14367,27 @@
       <c r="H67" s="12"/>
       <c r="I67" s="17"/>
       <c r="J67" s="17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L67" s="17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="M67" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>29</v>
@@ -14497,10 +14408,10 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Typos, spelling, and translations
</commit_message>
<xml_diff>
--- a/tools/game_levels.xlsx
+++ b/tools/game_levels.xlsx
@@ -672,13 +672,13 @@
     <t>notify_gov_statement_text</t>
   </si>
   <si>
-    <t>Die Folgen des Vulkanausbruchs sind stark spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, muss weiterhin und zu jeder Zeit die Spezialbrille getragen und täglich das Bad genommen werden. Diese Schutzmassnahmen sind für alle verpflichtend. Drücke "I" um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
-  </si>
-  <si>
-    <t>Die Folgen des Vulkanausbruchs sind weiterhin spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, wird weiterhin empfohlen, zu jeder Zeit die Spezialbrille zu tragen und täglich das Bad zu nehmen. Diese Schutzmassnahmen werden allen empfohlen. Drücke "I" um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
-  </si>
-  <si>
-    <t>Die Folgen des Vulkanausbruchs haben nachgelassen. Dennoch kann man sich immer noch infizieren, andere anstecken und sterben. Die Regierung hat diese Risiken gegen die Einschränkungen durch die Schutzmassnahmen abgewogen und gibt nun keine Empfehlungen mehr ab. Ob man die Spezialbrille trägt oder das tägliche Bad einnimmt, ist jedem Mika selbst überlassen. Drücke "I" um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B" um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
+    <t>Die Folgen des Vulkanausbruchs sind stark spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, muss weiterhin und zu jeder Zeit die Spezialbrille getragen und täglich das Bad genommen werden. Diese Schutzmassnahmen sind für alle verpflichtend. Drücke "I", um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B", um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
+  </si>
+  <si>
+    <t>Die Folgen des Vulkanausbruchs sind weiterhin spürbar: Viele Mikas haben sich infiziert und einige sind gestorben. Um sich selbst und andere Mikas zu schützen, wird weiterhin empfohlen, zu jeder Zeit die Spezialbrille zu tragen und täglich das Bad zu nehmen. Diese Schutzmassnahmen werden allen empfohlen. Drücke "I", um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B", um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
+  </si>
+  <si>
+    <t>Die Folgen des Vulkanausbruchs haben nachgelassen. Dennoch kann man sich immer noch infizieren, andere anstecken und sterben. Die Regierung hat diese Risiken gegen die Einschränkungen durch die Schutzmassnahmen abgewogen und gibt nun keine Empfehlungen mehr ab. Ob man die Spezialbrille trägt oder das tägliche Bad einnimmt, ist jedem Mika selbst überlassen. Drücke "I", um im Inventar deine Brille anzuziehen. In der Stadt findest du Wegschilder, die dich zum Badehaus leiten. Das Bad wirkt nur, wenn man es gesund nimmt. Drücke "B", um zu sehen, wie effektiv die Spezialbrille und das Bad sind, um vor der Vulkanseuche zu schützen.</t>
   </si>
   <si>
     <t>40% of ingroup NPCs wear a hat and a necklace; 60% wear only a hat</t>
@@ -6854,13 +6854,13 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J23:N23"/>
     <mergeCell ref="I24:N24"/>
     <mergeCell ref="I25:N25"/>
     <mergeCell ref="I26:N26"/>
     <mergeCell ref="I27:N27"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J23:N23"/>
     <mergeCell ref="I28:N28"/>
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
@@ -6902,22 +6902,22 @@
     <mergeCell ref="C30:H30"/>
     <mergeCell ref="C31:H31"/>
     <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C39:H39"/>
     <mergeCell ref="I43:N43"/>
     <mergeCell ref="J45:N45"/>
     <mergeCell ref="I46:N46"/>
     <mergeCell ref="I47:N47"/>
-    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="I67:N67"/>
+    <mergeCell ref="I68:N68"/>
     <mergeCell ref="C67:H67"/>
-    <mergeCell ref="I67:N67"/>
     <mergeCell ref="C68:H68"/>
-    <mergeCell ref="I68:N68"/>
-    <mergeCell ref="C39:H39"/>
     <mergeCell ref="C41:H41"/>
     <mergeCell ref="C43:H43"/>
     <mergeCell ref="C45:H45"/>
     <mergeCell ref="C46:H46"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C66:H66"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -12545,13 +12545,13 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J23:N23"/>
     <mergeCell ref="I25:N25"/>
     <mergeCell ref="I26:N26"/>
     <mergeCell ref="I27:N27"/>
     <mergeCell ref="I28:N28"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J23:N23"/>
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
@@ -18221,13 +18221,13 @@
     <mergeCell ref="I31:N31"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J23:N23"/>
     <mergeCell ref="I25:N25"/>
     <mergeCell ref="I26:N26"/>
     <mergeCell ref="I27:N27"/>
     <mergeCell ref="I28:N28"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J23:N23"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="C28:H28"/>
     <mergeCell ref="C29:H29"/>

</xml_diff>